<commit_message>
Big results push, waiting on protonet to finish
</commit_message>
<xml_diff>
--- a/fs_mol/outputs/test/plots/support_08/meanrank_Bacteria.xlsx
+++ b/fs_mol/outputs/test/plots/support_08/meanrank_Bacteria.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>meanrank</t>
   </si>
@@ -25,7 +25,13 @@
     <t>8_train (GNN-MT) val delta-auprc</t>
   </si>
   <si>
+    <t>8_train (GNN-MT-O) val delta-auprc</t>
+  </si>
+  <si>
     <t>8_train (PN) val delta-auprc</t>
+  </si>
+  <si>
+    <t>8_train (PN-O) val delta-auprc</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.214285714285714</v>
+        <v>3.442857142857143</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -407,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2.066666666666667</v>
+        <v>3.216666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -415,7 +421,23 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.585714285714286</v>
+        <v>3.016666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.642857142857143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2.285714285714286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>